<commit_message>
Problem with cumulative sums fixed
</commit_message>
<xml_diff>
--- a/OAS 2024.xlsx
+++ b/OAS 2024.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dnbar\Dropbox\OAS\OAS_Finances_2025\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dnbar\Dropbox\OAS\OAS_Finances_2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2487368A-9FBB-4D72-B8AF-717226F24E78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9544241F-B68A-48C1-9745-3D19BCA84E6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13695" firstSheet="2" activeTab="3" xr2:uid="{E6A7689A-682B-425D-92A3-B87F804748A5}"/>
+    <workbookView xWindow="4290" yWindow="3652" windowWidth="16200" windowHeight="9848" firstSheet="3" activeTab="8" xr2:uid="{E6A7689A-682B-425D-92A3-B87F804748A5}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="8" r:id="rId1"/>
@@ -36,8 +36,8 @@
   </definedNames>
   <calcPr calcId="191028"/>
   <pivotCaches>
-    <pivotCache cacheId="13" r:id="rId15"/>
-    <pivotCache cacheId="14" r:id="rId16"/>
+    <pivotCache cacheId="0" r:id="rId15"/>
+    <pivotCache cacheId="1" r:id="rId16"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9147" uniqueCount="3716">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9148" uniqueCount="3718">
   <si>
     <t>Subs</t>
   </si>
@@ -11207,6 +11207,12 @@
   </si>
   <si>
     <t>Commission on sales</t>
+  </si>
+  <si>
+    <t>#</t>
+  </si>
+  <si>
+    <t>Opening balance</t>
   </si>
 </sst>
 </file>
@@ -19990,7 +19996,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{A5C2633A-7AD5-4920-9B01-65373321B481}" name="PivotTable1" cacheId="14" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{A5C2633A-7AD5-4920-9B01-65373321B481}" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="E4:G8" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="9">
     <pivotField numFmtId="15" showAll="0"/>
@@ -20055,7 +20061,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{BE04C0F0-9A61-4F80-8276-3D04382D746D}" name="PivotTable2" cacheId="13" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{BE04C0F0-9A61-4F80-8276-3D04382D746D}" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:C29" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="8">
     <pivotField numFmtId="15" showAll="0"/>
@@ -20208,7 +20214,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{88CC6FF2-D2D5-4EC7-9086-AAE36B3B0E13}" name="PivotTable3" cacheId="14" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{88CC6FF2-D2D5-4EC7-9086-AAE36B3B0E13}" name="PivotTable3" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:C15" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="9">
     <pivotField numFmtId="15" showAll="0"/>
@@ -20330,7 +20336,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{2FE7C9AF-75EF-4873-8F1B-0F70A39EEC38}" name="PivotTable5" cacheId="14" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{2FE7C9AF-75EF-4873-8F1B-0F70A39EEC38}" name="PivotTable5" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A19:C31" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="9">
     <pivotField numFmtId="15" showAll="0"/>
@@ -21554,9 +21560,9 @@
         <v>90</v>
       </c>
       <c r="N23" s="18"/>
-      <c r="O23" s="36">
+      <c r="O23" s="36" t="e">
         <f>'Savings account'!F15+'Current account'!F400</f>
-        <v>28500.729999999996</v>
+        <v>#VALUE!</v>
       </c>
       <c r="S23" s="13">
         <f>SUM(S4:S6)-SUM(S10:S19)</f>
@@ -21730,9 +21736,9 @@
       <c r="L30" s="18"/>
       <c r="M30" s="18"/>
       <c r="N30" s="18"/>
-      <c r="O30" s="38">
+      <c r="O30" s="38" t="e">
         <f>O23</f>
-        <v>28500.729999999996</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="31" spans="1:22" ht="13.9" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
@@ -55180,8 +55186,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5956F534-76F9-4C2C-AE0C-5DBCF3D7B234}">
   <dimension ref="A1:I406"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -63244,9 +63250,8 @@
       <c r="E363">
         <v>30</v>
       </c>
-      <c r="F363" s="26">
-        <f t="shared" si="5"/>
-        <v>7010.2599999999957</v>
+      <c r="F363" s="26" t="s">
+        <v>3716</v>
       </c>
       <c r="G363" t="s">
         <v>3674</v>
@@ -63265,9 +63270,9 @@
       <c r="E364">
         <v>30</v>
       </c>
-      <c r="F364" s="26">
+      <c r="F364" s="26" t="e">
         <f t="shared" si="5"/>
-        <v>7040.2599999999957</v>
+        <v>#VALUE!</v>
       </c>
       <c r="G364" t="s">
         <v>3674</v>
@@ -63286,9 +63291,9 @@
       <c r="E365">
         <v>30</v>
       </c>
-      <c r="F365" s="26">
+      <c r="F365" s="26" t="e">
         <f t="shared" si="5"/>
-        <v>7070.2599999999957</v>
+        <v>#VALUE!</v>
       </c>
       <c r="G365" t="s">
         <v>3674</v>
@@ -63307,9 +63312,9 @@
       <c r="E366">
         <v>30</v>
       </c>
-      <c r="F366" s="26">
+      <c r="F366" s="26" t="e">
         <f t="shared" si="5"/>
-        <v>7100.2599999999957</v>
+        <v>#VALUE!</v>
       </c>
       <c r="G366" t="s">
         <v>3674</v>
@@ -63328,9 +63333,9 @@
       <c r="E367">
         <v>30</v>
       </c>
-      <c r="F367" s="26">
+      <c r="F367" s="26" t="e">
         <f t="shared" si="5"/>
-        <v>7130.2599999999957</v>
+        <v>#VALUE!</v>
       </c>
       <c r="G367" t="s">
         <v>3674</v>
@@ -63349,9 +63354,9 @@
       <c r="E368">
         <v>30</v>
       </c>
-      <c r="F368" s="26">
+      <c r="F368" s="26" t="e">
         <f t="shared" si="5"/>
-        <v>7160.2599999999957</v>
+        <v>#VALUE!</v>
       </c>
       <c r="G368" t="s">
         <v>3674</v>
@@ -63370,9 +63375,9 @@
       <c r="E369">
         <v>30</v>
       </c>
-      <c r="F369" s="26">
+      <c r="F369" s="26" t="e">
         <f t="shared" si="5"/>
-        <v>7190.2599999999957</v>
+        <v>#VALUE!</v>
       </c>
       <c r="G369" t="s">
         <v>3674</v>
@@ -63391,9 +63396,9 @@
       <c r="E370">
         <v>30</v>
       </c>
-      <c r="F370" s="26">
+      <c r="F370" s="26" t="e">
         <f t="shared" si="5"/>
-        <v>7220.2599999999957</v>
+        <v>#VALUE!</v>
       </c>
       <c r="G370" t="s">
         <v>3674</v>
@@ -63412,9 +63417,9 @@
       <c r="E371">
         <v>30</v>
       </c>
-      <c r="F371" s="26">
+      <c r="F371" s="26" t="e">
         <f t="shared" si="5"/>
-        <v>7250.2599999999957</v>
+        <v>#VALUE!</v>
       </c>
       <c r="G371" t="s">
         <v>3674</v>
@@ -63433,9 +63438,9 @@
       <c r="E372">
         <v>30</v>
       </c>
-      <c r="F372" s="26">
+      <c r="F372" s="26" t="e">
         <f t="shared" si="5"/>
-        <v>7280.2599999999957</v>
+        <v>#VALUE!</v>
       </c>
       <c r="G372" t="s">
         <v>3674</v>
@@ -63454,9 +63459,9 @@
       <c r="E373">
         <v>30</v>
       </c>
-      <c r="F373" s="26">
+      <c r="F373" s="26" t="e">
         <f t="shared" si="5"/>
-        <v>7310.2599999999957</v>
+        <v>#VALUE!</v>
       </c>
       <c r="G373" t="s">
         <v>3674</v>
@@ -63475,9 +63480,9 @@
       <c r="E374">
         <v>30</v>
       </c>
-      <c r="F374" s="26">
+      <c r="F374" s="26" t="e">
         <f t="shared" si="5"/>
-        <v>7340.2599999999957</v>
+        <v>#VALUE!</v>
       </c>
       <c r="G374" t="s">
         <v>3674</v>
@@ -63496,9 +63501,9 @@
       <c r="E375">
         <v>30</v>
       </c>
-      <c r="F375" s="26">
+      <c r="F375" s="26" t="e">
         <f t="shared" si="5"/>
-        <v>7370.2599999999957</v>
+        <v>#VALUE!</v>
       </c>
       <c r="G375" t="s">
         <v>3674</v>
@@ -63517,9 +63522,9 @@
       <c r="E376">
         <v>30</v>
       </c>
-      <c r="F376" s="26">
+      <c r="F376" s="26" t="e">
         <f t="shared" si="5"/>
-        <v>7400.2599999999957</v>
+        <v>#VALUE!</v>
       </c>
       <c r="G376" t="s">
         <v>3674</v>
@@ -63538,9 +63543,9 @@
       <c r="E377">
         <v>30</v>
       </c>
-      <c r="F377" s="26">
+      <c r="F377" s="26" t="e">
         <f t="shared" si="5"/>
-        <v>7430.2599999999957</v>
+        <v>#VALUE!</v>
       </c>
       <c r="G377" t="s">
         <v>3674</v>
@@ -63559,9 +63564,9 @@
       <c r="E378">
         <v>30</v>
       </c>
-      <c r="F378" s="26">
+      <c r="F378" s="26" t="e">
         <f t="shared" si="5"/>
-        <v>7460.2599999999957</v>
+        <v>#VALUE!</v>
       </c>
       <c r="G378" t="s">
         <v>3674</v>
@@ -63580,9 +63585,9 @@
       <c r="E379">
         <v>30</v>
       </c>
-      <c r="F379" s="26">
+      <c r="F379" s="26" t="e">
         <f t="shared" si="5"/>
-        <v>7490.2599999999957</v>
+        <v>#VALUE!</v>
       </c>
       <c r="G379" t="s">
         <v>3674</v>
@@ -63601,9 +63606,9 @@
       <c r="E380">
         <v>30</v>
       </c>
-      <c r="F380" s="26">
+      <c r="F380" s="26" t="e">
         <f t="shared" si="5"/>
-        <v>7520.2599999999957</v>
+        <v>#VALUE!</v>
       </c>
       <c r="G380" t="s">
         <v>3674</v>
@@ -63622,9 +63627,9 @@
       <c r="E381">
         <v>29.08</v>
       </c>
-      <c r="F381" s="26">
+      <c r="F381" s="26" t="e">
         <f t="shared" si="5"/>
-        <v>7549.3399999999956</v>
+        <v>#VALUE!</v>
       </c>
       <c r="G381" t="s">
         <v>3674</v>
@@ -63643,9 +63648,9 @@
       <c r="E382">
         <v>30</v>
       </c>
-      <c r="F382" s="26">
+      <c r="F382" s="26" t="e">
         <f t="shared" si="5"/>
-        <v>7579.3399999999956</v>
+        <v>#VALUE!</v>
       </c>
       <c r="G382" t="s">
         <v>3674</v>
@@ -63664,9 +63669,9 @@
       <c r="E383">
         <v>29.05</v>
       </c>
-      <c r="F383" s="26">
+      <c r="F383" s="26" t="e">
         <f t="shared" si="5"/>
-        <v>7608.3899999999958</v>
+        <v>#VALUE!</v>
       </c>
       <c r="G383" t="s">
         <v>3674</v>
@@ -63685,9 +63690,9 @@
       <c r="E384">
         <v>30</v>
       </c>
-      <c r="F384" s="26">
+      <c r="F384" s="26" t="e">
         <f t="shared" si="5"/>
-        <v>7638.3899999999958</v>
+        <v>#VALUE!</v>
       </c>
       <c r="G384" t="s">
         <v>3674</v>
@@ -63706,9 +63711,9 @@
       <c r="E385">
         <v>30</v>
       </c>
-      <c r="F385" s="26">
+      <c r="F385" s="26" t="e">
         <f t="shared" si="5"/>
-        <v>7668.3899999999958</v>
+        <v>#VALUE!</v>
       </c>
       <c r="G385" t="s">
         <v>3674</v>
@@ -63727,9 +63732,9 @@
       <c r="D386">
         <v>1157.28</v>
       </c>
-      <c r="F386" s="26">
+      <c r="F386" s="26" t="e">
         <f t="shared" si="5"/>
-        <v>6511.109999999996</v>
+        <v>#VALUE!</v>
       </c>
       <c r="G386" t="s">
         <v>789</v>
@@ -63751,9 +63756,9 @@
       <c r="D387">
         <v>6.05</v>
       </c>
-      <c r="F387" s="26">
+      <c r="F387" s="26" t="e">
         <f t="shared" si="5"/>
-        <v>6505.0599999999959</v>
+        <v>#VALUE!</v>
       </c>
       <c r="G387" t="s">
         <v>854</v>
@@ -63772,9 +63777,9 @@
       <c r="E388">
         <v>30</v>
       </c>
-      <c r="F388" s="26">
+      <c r="F388" s="26" t="e">
         <f t="shared" si="5"/>
-        <v>6535.0599999999959</v>
+        <v>#VALUE!</v>
       </c>
       <c r="G388" t="s">
         <v>3674</v>
@@ -63793,9 +63798,9 @@
       <c r="D389">
         <v>134.49</v>
       </c>
-      <c r="F389" s="26">
+      <c r="F389" s="26" t="e">
         <f t="shared" si="5"/>
-        <v>6400.5699999999961</v>
+        <v>#VALUE!</v>
       </c>
       <c r="G389" t="s">
         <v>737</v>
@@ -63817,9 +63822,9 @@
       <c r="D390">
         <v>750</v>
       </c>
-      <c r="F390" s="26">
+      <c r="F390" s="26" t="e">
         <f t="shared" ref="F390:F400" si="6">F389+E390-D390</f>
-        <v>5650.5699999999961</v>
+        <v>#VALUE!</v>
       </c>
       <c r="G390" t="s">
         <v>790</v>
@@ -63841,9 +63846,9 @@
       <c r="E391">
         <v>30</v>
       </c>
-      <c r="F391" s="26">
+      <c r="F391" s="26" t="e">
         <f t="shared" si="6"/>
-        <v>5680.5699999999961</v>
+        <v>#VALUE!</v>
       </c>
       <c r="G391" t="s">
         <v>3674</v>
@@ -63862,9 +63867,9 @@
       <c r="E392">
         <v>30</v>
       </c>
-      <c r="F392" s="26">
+      <c r="F392" s="26" t="e">
         <f t="shared" si="6"/>
-        <v>5710.5699999999961</v>
+        <v>#VALUE!</v>
       </c>
       <c r="G392" t="s">
         <v>3674</v>
@@ -63883,9 +63888,9 @@
       <c r="E393">
         <v>30</v>
       </c>
-      <c r="F393" s="26">
+      <c r="F393" s="26" t="e">
         <f t="shared" si="6"/>
-        <v>5740.5699999999961</v>
+        <v>#VALUE!</v>
       </c>
       <c r="G393" t="s">
         <v>3674</v>
@@ -63904,9 +63909,9 @@
       <c r="D394">
         <v>96.69</v>
       </c>
-      <c r="F394" s="26">
+      <c r="F394" s="26" t="e">
         <f t="shared" si="6"/>
-        <v>5643.8799999999965</v>
+        <v>#VALUE!</v>
       </c>
       <c r="G394" t="s">
         <v>737</v>
@@ -63928,9 +63933,9 @@
       <c r="E395">
         <v>30</v>
       </c>
-      <c r="F395" s="26">
+      <c r="F395" s="26" t="e">
         <f t="shared" si="6"/>
-        <v>5673.8799999999965</v>
+        <v>#VALUE!</v>
       </c>
       <c r="G395" t="s">
         <v>3674</v>
@@ -63949,9 +63954,9 @@
       <c r="E396">
         <v>30</v>
       </c>
-      <c r="F396" s="26">
+      <c r="F396" s="26" t="e">
         <f t="shared" si="6"/>
-        <v>5703.8799999999965</v>
+        <v>#VALUE!</v>
       </c>
       <c r="G396" t="s">
         <v>3674</v>
@@ -63970,9 +63975,9 @@
       <c r="E397">
         <v>30</v>
       </c>
-      <c r="F397" s="26">
+      <c r="F397" s="26" t="e">
         <f t="shared" si="6"/>
-        <v>5733.8799999999965</v>
+        <v>#VALUE!</v>
       </c>
       <c r="G397" t="s">
         <v>3674</v>
@@ -63991,9 +63996,9 @@
       <c r="E398">
         <v>30</v>
       </c>
-      <c r="F398" s="26">
+      <c r="F398" s="26" t="e">
         <f t="shared" si="6"/>
-        <v>5763.8799999999965</v>
+        <v>#VALUE!</v>
       </c>
       <c r="G398" t="s">
         <v>3674</v>
@@ -64012,9 +64017,9 @@
       <c r="E399">
         <v>30</v>
       </c>
-      <c r="F399" s="26">
+      <c r="F399" s="26" t="e">
         <f t="shared" si="6"/>
-        <v>5793.8799999999965</v>
+        <v>#VALUE!</v>
       </c>
       <c r="G399" t="s">
         <v>3674</v>
@@ -64033,9 +64038,9 @@
       <c r="E400">
         <v>30</v>
       </c>
-      <c r="F400" s="26">
+      <c r="F400" s="26" t="e">
         <f t="shared" si="6"/>
-        <v>5823.8799999999965</v>
+        <v>#VALUE!</v>
       </c>
       <c r="G400" t="s">
         <v>3674</v>
@@ -78429,15 +78434,15 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12A8BED0-6F25-4951-9707-565F124E30A4}">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3:E15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.53125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.796875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30.73046875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.19921875" style="29" bestFit="1" customWidth="1"/>
   </cols>
@@ -78466,6 +78471,12 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" s="3">
+        <v>45292</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3717</v>
+      </c>
       <c r="F2" s="29">
         <v>16329.34</v>
       </c>
@@ -78741,15 +78752,6 @@
       </c>
       <c r="G15" t="s">
         <v>92</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>2127</v>
-      </c>
-      <c r="E17">
-        <f>-SUM(E3:E15)</f>
-        <v>-6347.5099999999993</v>
       </c>
     </row>
   </sheetData>

</xml_diff>